<commit_message>
work on quality analysis
</commit_message>
<xml_diff>
--- a/Excel Files/ConfigFiles_all.xlsx
+++ b/Excel Files/ConfigFiles_all.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhiarzig\PycharmProjects\githubcrawler\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D55A17-C648-4D69-B5F2-85FBDEA3FEDD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F5E4329-7832-40FF-9060-F9DA5D011C1F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="17430" yWindow="-530" windowWidth="18000" windowHeight="9360" xr2:uid="{4D1D172B-2A50-47C6-8F79-D00F1A4E5A2C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4D1D172B-2A50-47C6-8F79-D00F1A4E5A2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -377,9 +377,6 @@
     <t>Clang</t>
   </si>
   <si>
-    <t>.clang*</t>
-  </si>
-  <si>
     <t>Codecov</t>
   </si>
   <si>
@@ -555,6 +552,9 @@
   </si>
   <si>
     <t>Azure Pipeline</t>
+  </si>
+  <si>
+    <t>.clang</t>
   </si>
 </sst>
 </file>
@@ -927,20 +927,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F99994D-A39A-4DA1-A607-129A152C2960}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" customWidth="1"/>
+    <col min="1" max="1" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" customWidth="1"/>
+    <col min="3" max="3" width="29.81640625" customWidth="1"/>
     <col min="4" max="4" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -954,7 +955,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -965,7 +966,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>107</v>
       </c>
@@ -973,230 +974,230 @@
         <v>112</v>
       </c>
       <c r="C3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B4" t="s">
-        <v>141</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" t="s">
+        <v>148</v>
+      </c>
+      <c r="C11" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>107</v>
+      </c>
+      <c r="B12" t="s">
+        <v>129</v>
+      </c>
+      <c r="C12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" t="s">
+        <v>129</v>
+      </c>
+      <c r="C14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16" t="s">
+        <v>133</v>
+      </c>
+      <c r="C16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>107</v>
+      </c>
+      <c r="B17" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B5" t="s">
-        <v>138</v>
-      </c>
-      <c r="C5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>107</v>
-      </c>
-      <c r="B6" t="s">
-        <v>138</v>
-      </c>
-      <c r="C6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>107</v>
-      </c>
-      <c r="B7" t="s">
-        <v>114</v>
-      </c>
-      <c r="C7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>107</v>
-      </c>
-      <c r="B8" t="s">
-        <v>116</v>
-      </c>
-      <c r="C8" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>107</v>
-      </c>
-      <c r="B9" t="s">
-        <v>118</v>
-      </c>
-      <c r="C9" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>107</v>
-      </c>
-      <c r="B10" t="s">
-        <v>120</v>
-      </c>
-      <c r="C10" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>107</v>
-      </c>
-      <c r="B11" t="s">
-        <v>149</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="C17" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>107</v>
+      </c>
+      <c r="B18" t="s">
+        <v>146</v>
+      </c>
+      <c r="C18" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>107</v>
+      </c>
+      <c r="B19" t="s">
+        <v>127</v>
+      </c>
+      <c r="C19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>107</v>
+      </c>
+      <c r="B20" t="s">
+        <v>123</v>
+      </c>
+      <c r="C20" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>107</v>
+      </c>
+      <c r="B21" t="s">
+        <v>135</v>
+      </c>
+      <c r="C21" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>107</v>
+      </c>
+      <c r="B22" t="s">
+        <v>125</v>
+      </c>
+      <c r="C22" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>107</v>
+      </c>
+      <c r="B23" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>107</v>
-      </c>
-      <c r="B12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>107</v>
-      </c>
-      <c r="B13" t="s">
-        <v>130</v>
-      </c>
-      <c r="C13" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>107</v>
-      </c>
-      <c r="B14" t="s">
-        <v>130</v>
-      </c>
-      <c r="C14" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>107</v>
-      </c>
-      <c r="B15" t="s">
-        <v>122</v>
-      </c>
-      <c r="C15" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>107</v>
-      </c>
-      <c r="B16" t="s">
-        <v>134</v>
-      </c>
-      <c r="C16" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>107</v>
-      </c>
-      <c r="B17" t="s">
-        <v>143</v>
-      </c>
-      <c r="C17" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>107</v>
-      </c>
-      <c r="B18" t="s">
-        <v>147</v>
-      </c>
-      <c r="C18" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>107</v>
-      </c>
-      <c r="B19" t="s">
-        <v>128</v>
-      </c>
-      <c r="C19" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>107</v>
-      </c>
-      <c r="B20" t="s">
-        <v>124</v>
-      </c>
-      <c r="C20" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>107</v>
-      </c>
-      <c r="B21" t="s">
-        <v>136</v>
-      </c>
-      <c r="C21" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>107</v>
-      </c>
-      <c r="B22" t="s">
-        <v>126</v>
-      </c>
-      <c r="C22" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>107</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>151</v>
       </c>
-      <c r="C23" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>107</v>
       </c>
@@ -1207,51 +1208,51 @@
         <v>109</v>
       </c>
     </row>
-    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>107</v>
       </c>
       <c r="B25" t="s">
+        <v>154</v>
+      </c>
+      <c r="C25" t="s">
         <v>155</v>
       </c>
-      <c r="C25" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>107</v>
       </c>
       <c r="B26" t="s">
+        <v>144</v>
+      </c>
+      <c r="C26" t="s">
         <v>145</v>
       </c>
-      <c r="C26" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>107</v>
       </c>
       <c r="B27" t="s">
+        <v>152</v>
+      </c>
+      <c r="C27" t="s">
         <v>153</v>
       </c>
-      <c r="C27" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>4</v>
       </c>
       <c r="B28" t="s">
+        <v>160</v>
+      </c>
+      <c r="C28" t="s">
         <v>161</v>
       </c>
-      <c r="C28" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -1262,7 +1263,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -1273,7 +1274,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -1284,18 +1285,18 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>4</v>
       </c>
       <c r="B32" t="s">
+        <v>156</v>
+      </c>
+      <c r="C32" t="s">
         <v>157</v>
       </c>
-      <c r="C32" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -1306,7 +1307,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -1317,18 +1318,18 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>4</v>
       </c>
       <c r="B35" t="s">
+        <v>162</v>
+      </c>
+      <c r="C35" t="s">
         <v>163</v>
       </c>
-      <c r="C35" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>4</v>
       </c>
@@ -1339,7 +1340,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -1350,7 +1351,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>4</v>
       </c>
@@ -1361,7 +1362,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>4</v>
       </c>
@@ -1372,7 +1373,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>4</v>
       </c>
@@ -1383,7 +1384,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>4</v>
       </c>
@@ -1397,7 +1398,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>4</v>
       </c>
@@ -1408,7 +1409,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>4</v>
       </c>
@@ -1419,7 +1420,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>4</v>
       </c>
@@ -1430,7 +1431,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>4</v>
       </c>
@@ -1441,7 +1442,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>4</v>
       </c>
@@ -1452,7 +1453,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>4</v>
       </c>
@@ -1466,7 +1467,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>4</v>
       </c>
@@ -1477,18 +1478,18 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>4</v>
       </c>
       <c r="B49" t="s">
+        <v>158</v>
+      </c>
+      <c r="C49" t="s">
         <v>159</v>
       </c>
-      <c r="C49" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>4</v>
       </c>
@@ -1499,7 +1500,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>4</v>
       </c>
@@ -1510,7 +1511,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>19</v>
       </c>
@@ -1521,12 +1522,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>19</v>
       </c>
       <c r="B53" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C53" t="s">
         <v>105</v>
@@ -1535,7 +1536,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>19</v>
       </c>
@@ -1546,7 +1547,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>19</v>
       </c>
@@ -1557,7 +1558,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>19</v>
       </c>
@@ -1571,7 +1572,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>19</v>
       </c>
@@ -1582,7 +1583,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>19</v>
       </c>
@@ -1593,7 +1594,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>19</v>
       </c>
@@ -1604,7 +1605,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>19</v>
       </c>
@@ -1615,7 +1616,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>19</v>
       </c>
@@ -1626,7 +1627,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>19</v>
       </c>
@@ -1637,7 +1638,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>19</v>
       </c>
@@ -1648,7 +1649,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>19</v>
       </c>
@@ -1659,18 +1660,18 @@
         <v>100</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B65" t="s">
+        <v>169</v>
+      </c>
+      <c r="C65" t="s">
         <v>170</v>
       </c>
-      <c r="C65" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>26</v>
       </c>
@@ -1681,7 +1682,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
         <v>26</v>
       </c>
@@ -1692,7 +1693,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
         <v>26</v>
       </c>
@@ -1703,7 +1704,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
         <v>26</v>
       </c>
@@ -1714,7 +1715,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
         <v>26</v>
       </c>
@@ -1725,7 +1726,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
         <v>26</v>
       </c>
@@ -1736,7 +1737,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
         <v>26</v>
       </c>
@@ -1744,10 +1745,10 @@
         <v>34</v>
       </c>
       <c r="C72" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
         <v>26</v>
       </c>
@@ -1755,10 +1756,10 @@
         <v>34</v>
       </c>
       <c r="C73" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
         <v>26</v>
       </c>
@@ -1769,7 +1770,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
         <v>26</v>
       </c>
@@ -1780,21 +1781,21 @@
         <v>39</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B76" t="s">
+        <v>166</v>
+      </c>
+      <c r="C76" t="s">
         <v>167</v>
       </c>
-      <c r="C76" t="s">
+      <c r="D76" t="s">
         <v>168</v>
       </c>
-      <c r="D76" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
         <v>26</v>
       </c>
@@ -1805,7 +1806,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
         <v>26</v>
       </c>
@@ -1816,7 +1817,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
         <v>26</v>
       </c>
@@ -1827,7 +1828,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
         <v>26</v>
       </c>
@@ -1838,7 +1839,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
         <v>26</v>
       </c>
@@ -1849,7 +1850,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>48</v>
       </c>
@@ -1860,7 +1861,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>48</v>
       </c>
@@ -1871,7 +1872,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>48</v>
       </c>
@@ -1882,7 +1883,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>48</v>
       </c>
@@ -1893,7 +1894,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>48</v>
       </c>
@@ -1904,7 +1905,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>48</v>
       </c>
@@ -1915,7 +1916,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>48</v>
       </c>
@@ -1926,7 +1927,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>48</v>
       </c>
@@ -1937,7 +1938,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>48</v>
       </c>
@@ -1948,7 +1949,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>48</v>
       </c>
@@ -1959,7 +1960,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>48</v>
       </c>
@@ -1973,7 +1974,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="93" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>48</v>
       </c>
@@ -1984,7 +1985,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="94" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>48</v>
       </c>
@@ -1996,13 +1997,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D94" xr:uid="{F11A2EA6-254C-4D97-ACCC-79A526040394}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Deployment automation"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:D94" xr:uid="{F11A2EA6-254C-4D97-ACCC-79A526040394}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D94">
     <sortCondition ref="A2:A94"/>
     <sortCondition ref="B2:B94"/>

</xml_diff>